<commit_message>
Fix: source delimiter issues
</commit_message>
<xml_diff>
--- a/data/src/electricity_footprint.xlsx
+++ b/data/src/electricity_footprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesse\Documents\code\carbon_guessr\code\data\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{130013A5-3A85-4C5B-B978-1FA2977CAFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8884D-7167-4D93-8C17-0A81E461F828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13920" tabRatio="587" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13920" tabRatio="587" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="210">
   <si>
     <t>id</t>
   </si>
@@ -675,6 +675,12 @@
   </si>
   <si>
     <t>Consuming 1 kWh of electricity requires *generating more* than 1 kWh because of losses occuring during transmission and distribution (T&amp;D losses, e.g. through the electricity grid). The amount of T&amp;D losses varies regionally as well. The carbon footprint value used here comes from the generation intensity of 2024 and the T&amp;D losses from 2014.</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -728,19 +734,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
@@ -787,11 +797,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F0CA2B46-DC38-4EC9-BDB2-D2C1368F28FF}" name="residential_intensity" displayName="residential_intensity" ref="A1:E154" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E154" xr:uid="{F0CA2B46-DC38-4EC9-BDB2-D2C1368F28FF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F9E10E12-0111-4880-9FB8-1692709759B5}" uniqueName="1" name="country" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{FCD6A8AF-B7BD-4F7B-9AEA-3BF8CD6C0EE2}" uniqueName="2" name="kgCO2eq_per_kWh" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{F9E10E12-0111-4880-9FB8-1692709759B5}" uniqueName="1" name="country" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FCD6A8AF-B7BD-4F7B-9AEA-3BF8CD6C0EE2}" uniqueName="2" name="kgCO2eq_per_kWh" queryTableFieldId="2" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{07CAB378-D158-4FC2-8FE0-84E3E4304435}" uniqueName="3" name="year_of_generation" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{B234A32E-21E3-474B-BDBD-8C5D222F5871}" uniqueName="4" name="year_of_td_losses" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{8DE689B4-39A2-4A03-8B06-D7C46CB3D1AD}" uniqueName="5" name="Column1" queryTableFieldId="5" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{8DE689B4-39A2-4A03-8B06-D7C46CB3D1AD}" uniqueName="5" name="Column1" queryTableFieldId="5" dataDxfId="3">
       <calculatedColumnFormula xml:space="preserve"> G$2 &amp; C2 &amp; G$3 &amp; D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -804,12 +814,12 @@
   <autoFilter ref="A1:G152" xr:uid="{F6ADF59C-B5EC-4703-A530-54EEE8FCC6C7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{45A886C0-C674-4AC9-8337-717B8C7CCBCB}" name="id"/>
-    <tableColumn id="2" xr3:uid="{DFBB2C40-BDE6-466D-B716-833545A1ECC4}" name="title" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{DFBB2C40-BDE6-466D-B716-833545A1ECC4}" name="title" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{E050B37F-592C-4A46-B27C-BA4963FFD560}" name="quantity"/>
     <tableColumn id="3" xr3:uid="{C0A046DA-D1BA-4495-80E4-8F862BB43A3E}" name="description"/>
-    <tableColumn id="4" xr3:uid="{E37DCBD3-75BB-4E21-AC4E-36CF22889050}" name="value" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{E37DCBD3-75BB-4E21-AC4E-36CF22889050}" name="value" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{096048CD-4F38-4473-B619-542187D30E01}" name="category"/>
-    <tableColumn id="6" xr3:uid="{4F53B61A-A1CD-42F0-9E05-9AA086B37D99}" name="sources"/>
+    <tableColumn id="6" xr3:uid="{4F53B61A-A1CD-42F0-9E05-9AA086B37D99}" name="sources" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1080,7 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DDD7B3-9F87-4867-B5F9-7A2411C23C3C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3940,8 +3950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3994,7 +4004,10 @@
       <c r="E2" s="3">
         <v>2.8287562148577094E-2</v>
       </c>
-      <c r="G2">
+      <c r="F2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4014,7 +4027,10 @@
       <c r="E3" s="3">
         <v>0.70106907112846706</v>
       </c>
-      <c r="G3">
+      <c r="F3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4034,7 +4050,10 @@
       <c r="E4" s="3">
         <v>0.18845736562808316</v>
       </c>
-      <c r="G4">
+      <c r="F4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4054,7 +4073,10 @@
       <c r="E5" s="3">
         <v>0.45158044394267877</v>
       </c>
-      <c r="G5">
+      <c r="F5" t="s">
+        <v>208</v>
+      </c>
+      <c r="G5" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4074,7 +4096,10 @@
       <c r="E6" s="3">
         <v>0.26156324298194528</v>
       </c>
-      <c r="G6">
+      <c r="F6" t="s">
+        <v>208</v>
+      </c>
+      <c r="G6" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4094,7 +4119,10 @@
       <c r="E7" s="3">
         <v>0.57776320311463891</v>
       </c>
-      <c r="G7">
+      <c r="F7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4114,7 +4142,10 @@
       <c r="E8" s="3">
         <v>0.10710640045842894</v>
       </c>
-      <c r="G8">
+      <c r="F8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4134,7 +4165,10 @@
       <c r="E9" s="3">
         <v>0.68458182708721238</v>
       </c>
-      <c r="G9">
+      <c r="F9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G9" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4154,7 +4188,10 @@
       <c r="E10" s="3">
         <v>0.93054594574647809</v>
       </c>
-      <c r="G10">
+      <c r="F10" t="s">
+        <v>208</v>
+      </c>
+      <c r="G10" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4174,7 +4211,10 @@
       <c r="E11" s="3">
         <v>0.75333227397024538</v>
       </c>
-      <c r="G11">
+      <c r="F11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G11" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4194,7 +4234,10 @@
       <c r="E12" s="3">
         <v>0.33655240691815336</v>
       </c>
-      <c r="G12">
+      <c r="F12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G12" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4214,7 +4257,10 @@
       <c r="E13" s="3">
         <v>0.12224844798216852</v>
       </c>
-      <c r="G13">
+      <c r="F13" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4234,7 +4280,10 @@
       <c r="E14" s="3">
         <v>0.95875000000000066</v>
       </c>
-      <c r="G14">
+      <c r="F14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G14" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4254,7 +4303,10 @@
       <c r="E15" s="3">
         <v>0.51446606375024084</v>
       </c>
-      <c r="G15">
+      <c r="F15" t="s">
+        <v>208</v>
+      </c>
+      <c r="G15" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4274,7 +4326,10 @@
       <c r="E16" s="3">
         <v>0.69139464521135141</v>
       </c>
-      <c r="G16">
+      <c r="F16" t="s">
+        <v>208</v>
+      </c>
+      <c r="G16" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4294,7 +4349,10 @@
       <c r="E17" s="3">
         <v>1.1208308923873644</v>
       </c>
-      <c r="G17">
+      <c r="F17" t="s">
+        <v>208</v>
+      </c>
+      <c r="G17" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4314,7 +4372,10 @@
       <c r="E18" s="3">
         <v>0.12158301627721867</v>
       </c>
-      <c r="G18">
+      <c r="F18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4334,7 +4395,10 @@
       <c r="E19" s="3">
         <v>0.98072397936850364</v>
       </c>
-      <c r="G19">
+      <c r="F19" t="s">
+        <v>208</v>
+      </c>
+      <c r="G19" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4354,7 +4418,10 @@
       <c r="E20" s="3">
         <v>0.27802583338160824</v>
       </c>
-      <c r="G20">
+      <c r="F20" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4374,7 +4441,10 @@
       <c r="E21" s="3">
         <v>0.63391529611909692</v>
       </c>
-      <c r="G21">
+      <c r="F21" t="s">
+        <v>208</v>
+      </c>
+      <c r="G21" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4394,7 +4464,10 @@
       <c r="E22" s="3">
         <v>0.57611504099902022</v>
       </c>
-      <c r="G22">
+      <c r="F22" t="s">
+        <v>208</v>
+      </c>
+      <c r="G22" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4414,7 +4487,10 @@
       <c r="E23" s="3">
         <v>0.36614601415906456</v>
       </c>
-      <c r="G23">
+      <c r="F23" t="s">
+        <v>208</v>
+      </c>
+      <c r="G23" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4434,7 +4510,10 @@
       <c r="E24" s="3">
         <v>0.18415223323420518</v>
       </c>
-      <c r="G24">
+      <c r="F24" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4454,7 +4533,10 @@
       <c r="E25" s="3">
         <v>0.8666090810486895</v>
       </c>
-      <c r="G25">
+      <c r="F25" t="s">
+        <v>208</v>
+      </c>
+      <c r="G25" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4474,7 +4556,10 @@
       <c r="E26" s="3">
         <v>0.27947795479863236</v>
       </c>
-      <c r="G26">
+      <c r="F26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G26" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4494,7 +4579,10 @@
       <c r="E27" s="3">
         <v>0.5793778143936823</v>
       </c>
-      <c r="G27">
+      <c r="F27" t="s">
+        <v>208</v>
+      </c>
+      <c r="G27" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4514,7 +4602,10 @@
       <c r="E28" s="3">
         <v>0.30934039376352113</v>
       </c>
-      <c r="G28">
+      <c r="F28" t="s">
+        <v>208</v>
+      </c>
+      <c r="G28" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4534,7 +4625,10 @@
       <c r="E29" s="3">
         <v>2.9732271096083635E-2</v>
       </c>
-      <c r="G29">
+      <c r="F29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G29" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4554,7 +4648,10 @@
       <c r="E30" s="3">
         <v>1.2879568143628515</v>
       </c>
-      <c r="G30">
+      <c r="F30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4574,7 +4671,10 @@
       <c r="E31" s="3">
         <v>6.8809760665070496E-2</v>
       </c>
-      <c r="G31">
+      <c r="F31" t="s">
+        <v>208</v>
+      </c>
+      <c r="G31" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4594,7 +4694,10 @@
       <c r="E32" s="3">
         <v>0.46275917893544743</v>
       </c>
-      <c r="G32">
+      <c r="F32" t="s">
+        <v>208</v>
+      </c>
+      <c r="G32" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4614,7 +4717,10 @@
       <c r="E33" s="3">
         <v>0.19752358867924535</v>
       </c>
-      <c r="G33">
+      <c r="F33" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4634,7 +4740,10 @@
       <c r="E34" s="3">
         <v>0.81863217818032663</v>
       </c>
-      <c r="G34">
+      <c r="F34" t="s">
+        <v>208</v>
+      </c>
+      <c r="G34" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4654,7 +4763,10 @@
       <c r="E35" s="3">
         <v>0.52653327334113964</v>
       </c>
-      <c r="G35">
+      <c r="F35" t="s">
+        <v>208</v>
+      </c>
+      <c r="G35" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4674,7 +4786,10 @@
       <c r="E36" s="3">
         <v>0.43065153569032638</v>
       </c>
-      <c r="G36">
+      <c r="F36" t="s">
+        <v>208</v>
+      </c>
+      <c r="G36" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4694,7 +4809,10 @@
       <c r="E37" s="3">
         <v>0.15144071528122763</v>
       </c>
-      <c r="G37">
+      <c r="F37" t="s">
+        <v>208</v>
+      </c>
+      <c r="G37" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4714,7 +4832,10 @@
       <c r="E38" s="3">
         <v>0.62953019367252727</v>
       </c>
-      <c r="G38">
+      <c r="F38" t="s">
+        <v>208</v>
+      </c>
+      <c r="G38" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4734,7 +4855,10 @@
       <c r="E39" s="3">
         <v>0.24673574718710997</v>
       </c>
-      <c r="G39">
+      <c r="F39" t="s">
+        <v>208</v>
+      </c>
+      <c r="G39" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4754,7 +4878,10 @@
       <c r="E40" s="3">
         <v>0.73271159284692833</v>
       </c>
-      <c r="G40">
+      <c r="F40" t="s">
+        <v>208</v>
+      </c>
+      <c r="G40" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4774,7 +4901,10 @@
       <c r="E41" s="3">
         <v>0.11362140142813867</v>
       </c>
-      <c r="G41">
+      <c r="F41" t="s">
+        <v>208</v>
+      </c>
+      <c r="G41" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4794,7 +4924,10 @@
       <c r="E42" s="3">
         <v>0.67898653648548046</v>
       </c>
-      <c r="G42">
+      <c r="F42" t="s">
+        <v>208</v>
+      </c>
+      <c r="G42" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4814,7 +4947,10 @@
       <c r="E43" s="3">
         <v>0.67556651845272198</v>
       </c>
-      <c r="G43">
+      <c r="F43" t="s">
+        <v>208</v>
+      </c>
+      <c r="G43" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4834,7 +4970,10 @@
       <c r="E44" s="3">
         <v>0.42305147653619074</v>
       </c>
-      <c r="G44">
+      <c r="F44" t="s">
+        <v>208</v>
+      </c>
+      <c r="G44" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4854,7 +4993,10 @@
       <c r="E45" s="3">
         <v>0.19418674813852821</v>
       </c>
-      <c r="G45">
+      <c r="F45" t="s">
+        <v>208</v>
+      </c>
+      <c r="G45" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4874,7 +5016,10 @@
       <c r="E46" s="3">
         <v>3.0606300908545735E-2</v>
       </c>
-      <c r="G46">
+      <c r="F46" t="s">
+        <v>208</v>
+      </c>
+      <c r="G46" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4894,7 +5039,10 @@
       <c r="E47" s="3">
         <v>7.4744649210012878E-2</v>
       </c>
-      <c r="G47">
+      <c r="F47" t="s">
+        <v>208</v>
+      </c>
+      <c r="G47" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4914,7 +5062,10 @@
       <c r="E48" s="3">
         <v>4.7394050251367933E-2</v>
       </c>
-      <c r="G48">
+      <c r="F48" t="s">
+        <v>208</v>
+      </c>
+      <c r="G48" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4934,7 +5085,10 @@
       <c r="E49" s="3">
         <v>0.52949358340672059</v>
       </c>
-      <c r="G49">
+      <c r="F49" t="s">
+        <v>208</v>
+      </c>
+      <c r="G49" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4954,7 +5108,10 @@
       <c r="E50" s="3">
         <v>0.15544177751506372</v>
       </c>
-      <c r="G50">
+      <c r="F50" t="s">
+        <v>208</v>
+      </c>
+      <c r="G50" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4974,7 +5131,10 @@
       <c r="E51" s="3">
         <v>0.36208678733898658</v>
       </c>
-      <c r="G51">
+      <c r="F51" t="s">
+        <v>208</v>
+      </c>
+      <c r="G51" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -4994,7 +5154,10 @@
       <c r="E52" s="3">
         <v>0.51195219572927331</v>
       </c>
-      <c r="G52">
+      <c r="F52" t="s">
+        <v>208</v>
+      </c>
+      <c r="G52" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5014,7 +5177,10 @@
       <c r="E53" s="3">
         <v>0.60828873823529406</v>
       </c>
-      <c r="G53">
+      <c r="F53" t="s">
+        <v>208</v>
+      </c>
+      <c r="G53" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5034,7 +5200,10 @@
       <c r="E54" s="3">
         <v>0.36020451800137226</v>
       </c>
-      <c r="G54">
+      <c r="F54" t="s">
+        <v>208</v>
+      </c>
+      <c r="G54" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5054,7 +5223,10 @@
       <c r="E55" s="3">
         <v>0.31309126609206311</v>
       </c>
-      <c r="G55">
+      <c r="F55" t="s">
+        <v>208</v>
+      </c>
+      <c r="G55" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5074,7 +5246,10 @@
       <c r="E56" s="3">
         <v>0.62841967711962843</v>
       </c>
-      <c r="G56">
+      <c r="F56" t="s">
+        <v>208</v>
+      </c>
+      <c r="G56" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5094,7 +5269,10 @@
       <c r="E57" s="3">
         <v>0.42477157549793049</v>
       </c>
-      <c r="G57">
+      <c r="F57" t="s">
+        <v>208</v>
+      </c>
+      <c r="G57" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5114,7 +5292,10 @@
       <c r="E58" s="3">
         <v>0.7139495200916447</v>
       </c>
-      <c r="G58">
+      <c r="F58" t="s">
+        <v>208</v>
+      </c>
+      <c r="G58" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5134,7 +5315,10 @@
       <c r="E59" s="3">
         <v>0.19651852002179176</v>
       </c>
-      <c r="G59">
+      <c r="F59" t="s">
+        <v>208</v>
+      </c>
+      <c r="G59" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5154,7 +5338,10 @@
       <c r="E60" s="3">
         <v>2.9110892112538075E-2</v>
       </c>
-      <c r="G60">
+      <c r="F60" t="s">
+        <v>208</v>
+      </c>
+      <c r="G60" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5174,7 +5361,10 @@
       <c r="E61" s="3">
         <v>0.83735748664837206</v>
       </c>
-      <c r="G61">
+      <c r="F61" t="s">
+        <v>208</v>
+      </c>
+      <c r="G61" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5194,7 +5384,10 @@
       <c r="E62" s="3">
         <v>0.73520073487887372</v>
       </c>
-      <c r="G62">
+      <c r="F62" t="s">
+        <v>208</v>
+      </c>
+      <c r="G62" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5214,7 +5407,10 @@
       <c r="E63" s="3">
         <v>0.7136033488469633</v>
       </c>
-      <c r="G63">
+      <c r="F63" t="s">
+        <v>208</v>
+      </c>
+      <c r="G63" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5234,7 +5430,10 @@
       <c r="E64" s="3">
         <v>1.6916374565640804</v>
       </c>
-      <c r="G64">
+      <c r="F64" t="s">
+        <v>208</v>
+      </c>
+      <c r="G64" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5254,7 +5453,10 @@
       <c r="E65" s="3">
         <v>0.30381059590262144</v>
       </c>
-      <c r="G65">
+      <c r="F65" t="s">
+        <v>208</v>
+      </c>
+      <c r="G65" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5274,7 +5476,10 @@
       <c r="E66" s="3">
         <v>0.59509158608537027</v>
       </c>
-      <c r="G66">
+      <c r="F66" t="s">
+        <v>208</v>
+      </c>
+      <c r="G66" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5294,7 +5499,10 @@
       <c r="E67" s="3">
         <v>0.30807385535752663</v>
       </c>
-      <c r="G67">
+      <c r="F67" t="s">
+        <v>208</v>
+      </c>
+      <c r="G67" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5314,7 +5522,10 @@
       <c r="E68" s="3">
         <v>0.76469507143953308</v>
       </c>
-      <c r="G68">
+      <c r="F68" t="s">
+        <v>208</v>
+      </c>
+      <c r="G68" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5334,7 +5545,10 @@
       <c r="E69" s="3">
         <v>0.50318141563253804</v>
       </c>
-      <c r="G69">
+      <c r="F69" t="s">
+        <v>208</v>
+      </c>
+      <c r="G69" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5354,7 +5568,10 @@
       <c r="E70" s="3">
         <v>0.60557583507692281</v>
       </c>
-      <c r="G70">
+      <c r="F70" t="s">
+        <v>208</v>
+      </c>
+      <c r="G70" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5374,7 +5591,10 @@
       <c r="E71" s="3">
         <v>0.87423397330722052</v>
       </c>
-      <c r="G71">
+      <c r="F71" t="s">
+        <v>208</v>
+      </c>
+      <c r="G71" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5394,7 +5614,10 @@
       <c r="E72" s="3">
         <v>0.11184666475140131</v>
       </c>
-      <c r="G72">
+      <c r="F72" t="s">
+        <v>208</v>
+      </c>
+      <c r="G72" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5414,7 +5637,10 @@
       <c r="E73" s="3">
         <v>0.40738412092872484</v>
       </c>
-      <c r="G73">
+      <c r="F73" t="s">
+        <v>208</v>
+      </c>
+      <c r="G73" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5434,7 +5660,10 @@
       <c r="E74" s="3">
         <v>0.42832211514342056</v>
       </c>
-      <c r="G74">
+      <c r="F74" t="s">
+        <v>208</v>
+      </c>
+      <c r="G74" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5454,7 +5683,10 @@
       <c r="E75" s="3">
         <v>1.1285221249860886</v>
       </c>
-      <c r="G75">
+      <c r="F75" t="s">
+        <v>208</v>
+      </c>
+      <c r="G75" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5474,7 +5706,10 @@
       <c r="E76" s="3">
         <v>0.70000051435919686</v>
       </c>
-      <c r="G76">
+      <c r="F76" t="s">
+        <v>208</v>
+      </c>
+      <c r="G76" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5494,7 +5729,10 @@
       <c r="E77" s="3">
         <v>0.19771169773273017</v>
       </c>
-      <c r="G77">
+      <c r="F77" t="s">
+        <v>208</v>
+      </c>
+      <c r="G77" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5514,7 +5752,10 @@
       <c r="E78" s="3">
         <v>0.24351281090740892</v>
       </c>
-      <c r="G78">
+      <c r="F78" t="s">
+        <v>208</v>
+      </c>
+      <c r="G78" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5534,7 +5775,10 @@
       <c r="E79" s="3">
         <v>0.14479211017473786</v>
       </c>
-      <c r="G79">
+      <c r="F79" t="s">
+        <v>208</v>
+      </c>
+      <c r="G79" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5554,7 +5798,10 @@
       <c r="E80" s="3">
         <v>0.40943970937595908</v>
       </c>
-      <c r="G80">
+      <c r="F80" t="s">
+        <v>208</v>
+      </c>
+      <c r="G80" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5574,7 +5821,10 @@
       <c r="E81" s="3">
         <v>1.0403809975236398</v>
       </c>
-      <c r="G81">
+      <c r="F81" t="s">
+        <v>208</v>
+      </c>
+      <c r="G81" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5594,7 +5844,10 @@
       <c r="E82" s="3">
         <v>0.16209377826425378</v>
       </c>
-      <c r="G82">
+      <c r="F82" t="s">
+        <v>208</v>
+      </c>
+      <c r="G82" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5614,7 +5867,10 @@
       <c r="E83" s="3">
         <v>0.14356572159750108</v>
       </c>
-      <c r="G83">
+      <c r="F83" t="s">
+        <v>208</v>
+      </c>
+      <c r="G83" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5634,7 +5890,10 @@
       <c r="E84" s="3">
         <v>0.50388426872727266</v>
       </c>
-      <c r="G84">
+      <c r="F84" t="s">
+        <v>208</v>
+      </c>
+      <c r="G84" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5654,7 +5913,10 @@
       <c r="E85" s="3">
         <v>0.64920528593416671</v>
       </c>
-      <c r="G85">
+      <c r="F85" t="s">
+        <v>208</v>
+      </c>
+      <c r="G85" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5674,7 +5936,10 @@
       <c r="E86" s="3">
         <v>0.52640375993361788</v>
       </c>
-      <c r="G86">
+      <c r="F86" t="s">
+        <v>208</v>
+      </c>
+      <c r="G86" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5694,7 +5959,10 @@
       <c r="E87" s="3">
         <v>0.66997379453681716</v>
       </c>
-      <c r="G87">
+      <c r="F87" t="s">
+        <v>208</v>
+      </c>
+      <c r="G87" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5714,7 +5982,10 @@
       <c r="E88" s="3">
         <v>0.55023654156879498</v>
       </c>
-      <c r="G88">
+      <c r="F88" t="s">
+        <v>208</v>
+      </c>
+      <c r="G88" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5734,7 +6005,10 @@
       <c r="E89" s="3">
         <v>0.70643093997894768</v>
       </c>
-      <c r="G89">
+      <c r="F89" t="s">
+        <v>208</v>
+      </c>
+      <c r="G89" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5754,7 +6028,10 @@
       <c r="E90" s="3">
         <v>0.91246048956299741</v>
       </c>
-      <c r="G90">
+      <c r="F90" t="s">
+        <v>208</v>
+      </c>
+      <c r="G90" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5774,7 +6051,10 @@
       <c r="E91" s="3">
         <v>0.48284423444639746</v>
       </c>
-      <c r="G91">
+      <c r="F91" t="s">
+        <v>208</v>
+      </c>
+      <c r="G91" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5794,7 +6074,10 @@
       <c r="E92" s="3">
         <v>0.70266821258506296</v>
       </c>
-      <c r="G92">
+      <c r="F92" t="s">
+        <v>208</v>
+      </c>
+      <c r="G92" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5814,7 +6097,10 @@
       <c r="E93" s="3">
         <v>0.15450550426231541</v>
       </c>
-      <c r="G93">
+      <c r="F93" t="s">
+        <v>208</v>
+      </c>
+      <c r="G93" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5834,7 +6120,10 @@
       <c r="E94" s="3">
         <v>0.61937730497920995</v>
       </c>
-      <c r="G94">
+      <c r="F94" t="s">
+        <v>208</v>
+      </c>
+      <c r="G94" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5854,7 +6143,10 @@
       <c r="E95" s="3">
         <v>7.8344815265760245E-2</v>
       </c>
-      <c r="G95">
+      <c r="F95" t="s">
+        <v>208</v>
+      </c>
+      <c r="G95" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5874,7 +6166,10 @@
       <c r="E96" s="3">
         <v>2.7591928699547127E-2</v>
       </c>
-      <c r="G96">
+      <c r="F96" t="s">
+        <v>208</v>
+      </c>
+      <c r="G96" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5894,7 +6189,10 @@
       <c r="E97" s="3">
         <v>0.26389960788507938</v>
       </c>
-      <c r="G97">
+      <c r="F97" t="s">
+        <v>208</v>
+      </c>
+      <c r="G97" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5914,7 +6212,10 @@
       <c r="E98" s="3">
         <v>0.12932788842615361</v>
       </c>
-      <c r="G98">
+      <c r="F98" t="s">
+        <v>208</v>
+      </c>
+      <c r="G98" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5934,7 +6235,10 @@
       <c r="E99" s="3">
         <v>0.35675777869442082</v>
       </c>
-      <c r="G99">
+      <c r="F99" t="s">
+        <v>208</v>
+      </c>
+      <c r="G99" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5954,7 +6258,10 @@
       <c r="E100" s="3">
         <v>1.289268585131895</v>
       </c>
-      <c r="G100">
+      <c r="F100" t="s">
+        <v>208</v>
+      </c>
+      <c r="G100" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5974,7 +6281,10 @@
       <c r="E101" s="3">
         <v>0.59108276878376698</v>
       </c>
-      <c r="G101">
+      <c r="F101" t="s">
+        <v>208</v>
+      </c>
+      <c r="G101" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -5994,7 +6304,10 @@
       <c r="E102" s="3">
         <v>0.680441909191695</v>
       </c>
-      <c r="G102">
+      <c r="F102" t="s">
+        <v>208</v>
+      </c>
+      <c r="G102" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6014,7 +6327,10 @@
       <c r="E103" s="3">
         <v>3.2273913032766555E-2</v>
       </c>
-      <c r="G103">
+      <c r="F103" t="s">
+        <v>208</v>
+      </c>
+      <c r="G103" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6034,7 +6350,10 @@
       <c r="E104" s="3">
         <v>0.60445889907326311</v>
       </c>
-      <c r="G104">
+      <c r="F104" t="s">
+        <v>208</v>
+      </c>
+      <c r="G104" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6054,7 +6373,10 @@
       <c r="E105" s="3">
         <v>0.46803275134404232</v>
       </c>
-      <c r="G105">
+      <c r="F105" t="s">
+        <v>208</v>
+      </c>
+      <c r="G105" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6074,7 +6396,10 @@
       <c r="E106" s="3">
         <v>0.27875475196409716</v>
       </c>
-      <c r="G106">
+      <c r="F106" t="s">
+        <v>208</v>
+      </c>
+      <c r="G106" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6094,7 +6419,10 @@
       <c r="E107" s="3">
         <v>2.8182309615171139E-2</v>
       </c>
-      <c r="G107">
+      <c r="F107" t="s">
+        <v>208</v>
+      </c>
+      <c r="G107" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6114,7 +6442,10 @@
       <c r="E108" s="3">
         <v>0.29614406785781483</v>
       </c>
-      <c r="G108">
+      <c r="F108" t="s">
+        <v>208</v>
+      </c>
+      <c r="G108" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6134,7 +6465,10 @@
       <c r="E109" s="3">
         <v>0.67843391332348102</v>
       </c>
-      <c r="G109">
+      <c r="F109" t="s">
+        <v>208</v>
+      </c>
+      <c r="G109" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6154,7 +6488,10 @@
       <c r="E110" s="3">
         <v>0.65572871945175282</v>
       </c>
-      <c r="G110">
+      <c r="F110" t="s">
+        <v>208</v>
+      </c>
+      <c r="G110" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6174,7 +6511,10 @@
       <c r="E111" s="3">
         <v>0.12443768621570225</v>
       </c>
-      <c r="G111">
+      <c r="F111" t="s">
+        <v>208</v>
+      </c>
+      <c r="G111" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6194,7 +6534,10 @@
       <c r="E112" s="3">
         <v>0.63936209833404523</v>
       </c>
-      <c r="G112">
+      <c r="F112" t="s">
+        <v>208</v>
+      </c>
+      <c r="G112" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6214,7 +6557,10 @@
       <c r="E113" s="3">
         <v>0.27208663834431451</v>
       </c>
-      <c r="G113">
+      <c r="F113" t="s">
+        <v>208</v>
+      </c>
+      <c r="G113" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6234,7 +6580,10 @@
       <c r="E114" s="3">
         <v>0.49122849298925103</v>
       </c>
-      <c r="G114">
+      <c r="F114" t="s">
+        <v>208</v>
+      </c>
+      <c r="G114" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6254,7 +6603,10 @@
       <c r="E115" s="3">
         <v>0.36645795678059534</v>
       </c>
-      <c r="G115">
+      <c r="F115" t="s">
+        <v>208</v>
+      </c>
+      <c r="G115" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6274,7 +6626,10 @@
       <c r="E116" s="3">
         <v>0.76577318825528828</v>
       </c>
-      <c r="G116">
+      <c r="F116" t="s">
+        <v>208</v>
+      </c>
+      <c r="G116" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6294,7 +6649,10 @@
       <c r="E117" s="3">
         <v>0.61555932551020398</v>
       </c>
-      <c r="G117">
+      <c r="F117" t="s">
+        <v>208</v>
+      </c>
+      <c r="G117" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6314,7 +6672,10 @@
       <c r="E118" s="3">
         <v>0.76031841661080801</v>
       </c>
-      <c r="G118">
+      <c r="F118" t="s">
+        <v>208</v>
+      </c>
+      <c r="G118" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6334,7 +6695,10 @@
       <c r="E119" s="3">
         <v>0.50022463903146253</v>
       </c>
-      <c r="G119">
+      <c r="F119" t="s">
+        <v>208</v>
+      </c>
+      <c r="G119" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6354,7 +6718,10 @@
       <c r="E120" s="3">
         <v>0.10131998828325725</v>
       </c>
-      <c r="G120">
+      <c r="F120" t="s">
+        <v>208</v>
+      </c>
+      <c r="G120" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6374,7 +6741,10 @@
       <c r="E121" s="3">
         <v>0.23915947798502563</v>
       </c>
-      <c r="G121">
+      <c r="F121" t="s">
+        <v>208</v>
+      </c>
+      <c r="G121" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6394,7 +6764,10 @@
       <c r="E122" s="3">
         <v>0.78911118385939272</v>
       </c>
-      <c r="G122">
+      <c r="F122" t="s">
+        <v>208</v>
+      </c>
+      <c r="G122" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6414,7 +6787,10 @@
       <c r="E123" s="3">
         <v>0.63495401021276598</v>
       </c>
-      <c r="G123">
+      <c r="F123" t="s">
+        <v>208</v>
+      </c>
+      <c r="G123" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6434,7 +6810,10 @@
       <c r="E124" s="3">
         <v>0.15984919291789562</v>
       </c>
-      <c r="G124">
+      <c r="F124" t="s">
+        <v>208</v>
+      </c>
+      <c r="G124" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6454,7 +6833,10 @@
       <c r="E125" s="3">
         <v>0.55691926376589995</v>
       </c>
-      <c r="G125">
+      <c r="F125" t="s">
+        <v>208</v>
+      </c>
+      <c r="G125" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6474,7 +6856,10 @@
       <c r="E126" s="3">
         <v>0.27504473779096816</v>
       </c>
-      <c r="G126">
+      <c r="F126" t="s">
+        <v>208</v>
+      </c>
+      <c r="G126" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6494,7 +6879,10 @@
       <c r="E127" s="3">
         <v>0.43351900879478833</v>
       </c>
-      <c r="G127">
+      <c r="F127" t="s">
+        <v>208</v>
+      </c>
+      <c r="G127" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6514,7 +6902,10 @@
       <c r="E128" s="3">
         <v>3.8021836425190102E-2</v>
       </c>
-      <c r="G128">
+      <c r="F128" t="s">
+        <v>208</v>
+      </c>
+      <c r="G128" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6534,7 +6925,10 @@
       <c r="E129" s="3">
         <v>3.8821240441737931E-2</v>
       </c>
-      <c r="G129">
+      <c r="F129" t="s">
+        <v>208</v>
+      </c>
+      <c r="G129" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6554,7 +6948,10 @@
       <c r="E130" s="3">
         <v>0.8636444552839474</v>
       </c>
-      <c r="G130">
+      <c r="F130" t="s">
+        <v>208</v>
+      </c>
+      <c r="G130" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6574,7 +6971,10 @@
       <c r="E131" s="3">
         <v>0.14172968975698585</v>
       </c>
-      <c r="G131">
+      <c r="F131" t="s">
+        <v>208</v>
+      </c>
+      <c r="G131" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6594,7 +6994,10 @@
       <c r="E132" s="3">
         <v>0.45630300204133728</v>
       </c>
-      <c r="G132">
+      <c r="F132" t="s">
+        <v>208</v>
+      </c>
+      <c r="G132" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6614,7 +7017,10 @@
       <c r="E133" s="3">
         <v>0.59855847635675563</v>
       </c>
-      <c r="G133">
+      <c r="F133" t="s">
+        <v>208</v>
+      </c>
+      <c r="G133" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6634,7 +7040,10 @@
       <c r="E134" s="3">
         <v>0.63458560711974099</v>
       </c>
-      <c r="G134">
+      <c r="F134" t="s">
+        <v>208</v>
+      </c>
+      <c r="G134" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6654,7 +7063,10 @@
       <c r="E135" s="3">
         <v>0.71930966595201073</v>
       </c>
-      <c r="G135">
+      <c r="F135" t="s">
+        <v>208</v>
+      </c>
+      <c r="G135" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6674,7 +7086,10 @@
       <c r="E136" s="3">
         <v>0.71591908696373152</v>
       </c>
-      <c r="G136">
+      <c r="F136" t="s">
+        <v>208</v>
+      </c>
+      <c r="G136" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6694,7 +7109,10 @@
       <c r="E137" s="3">
         <v>0.51680480984158239</v>
       </c>
-      <c r="G137">
+      <c r="F137" t="s">
+        <v>208</v>
+      </c>
+      <c r="G137" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6714,7 +7132,10 @@
       <c r="E138" s="3">
         <v>1.4457325285171101</v>
       </c>
-      <c r="G138">
+      <c r="F138" t="s">
+        <v>208</v>
+      </c>
+      <c r="G138" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6734,7 +7155,10 @@
       <c r="E139" s="3">
         <v>7.1138614230521549E-2</v>
       </c>
-      <c r="G139">
+      <c r="F139" t="s">
+        <v>208</v>
+      </c>
+      <c r="G139" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6754,7 +7178,10 @@
       <c r="E140" s="3">
         <v>0.28434268602031831</v>
       </c>
-      <c r="G140">
+      <c r="F140" t="s">
+        <v>208</v>
+      </c>
+      <c r="G140" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6774,7 +7201,10 @@
       <c r="E141" s="3">
         <v>0.5171452069164697</v>
       </c>
-      <c r="G141">
+      <c r="F141" t="s">
+        <v>208</v>
+      </c>
+      <c r="G141" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6794,7 +7224,10 @@
       <c r="E142" s="3">
         <v>0.23212321534023686</v>
       </c>
-      <c r="G142">
+      <c r="F142" t="s">
+        <v>208</v>
+      </c>
+      <c r="G142" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6814,7 +7247,10 @@
       <c r="E143" s="3">
         <v>0.40161200765507943</v>
       </c>
-      <c r="G143">
+      <c r="F143" t="s">
+        <v>208</v>
+      </c>
+      <c r="G143" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6834,7 +7270,10 @@
       <c r="E144" s="3">
         <v>0.10605725226640013</v>
       </c>
-      <c r="G144">
+      <c r="F144" t="s">
+        <v>208</v>
+      </c>
+      <c r="G144" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6854,7 +7293,10 @@
       <c r="E145" s="3">
         <v>1.1746218042135703</v>
       </c>
-      <c r="G145">
+      <c r="F145" t="s">
+        <v>208</v>
+      </c>
+      <c r="G145" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6874,7 +7316,10 @@
       <c r="E146" s="3">
         <v>0.26175567382652981</v>
       </c>
-      <c r="G146">
+      <c r="F146" t="s">
+        <v>208</v>
+      </c>
+      <c r="G146" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6894,7 +7339,10 @@
       <c r="E147" s="3">
         <v>0.50229777570626355</v>
       </c>
-      <c r="G147">
+      <c r="F147" t="s">
+        <v>208</v>
+      </c>
+      <c r="G147" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6914,7 +7362,10 @@
       <c r="E148" s="3">
         <v>0.50390813992867023</v>
       </c>
-      <c r="G148">
+      <c r="F148" t="s">
+        <v>209</v>
+      </c>
+      <c r="G148" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6934,7 +7385,10 @@
       <c r="E149" s="3">
         <v>0.72302280407174013</v>
       </c>
-      <c r="G149">
+      <c r="F149" t="s">
+        <v>208</v>
+      </c>
+      <c r="G149" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6954,7 +7408,10 @@
       <c r="E150" s="3">
         <v>0.12536479234326967</v>
       </c>
-      <c r="G150">
+      <c r="F150" t="s">
+        <v>208</v>
+      </c>
+      <c r="G150" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6974,7 +7431,10 @@
       <c r="E151" s="3">
         <v>0.38497263796117953</v>
       </c>
-      <c r="G151">
+      <c r="F151" t="s">
+        <v>208</v>
+      </c>
+      <c r="G151" s="4">
         <v>1.2</v>
       </c>
     </row>
@@ -6994,7 +7454,10 @@
       <c r="E152" s="3">
         <v>0.253077</v>
       </c>
-      <c r="G152">
+      <c r="F152" t="s">
+        <v>209</v>
+      </c>
+      <c r="G152" s="4">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>